<commit_message>
data update in excel
</commit_message>
<xml_diff>
--- a/analysis/failedTestDetails.xlsx
+++ b/analysis/failedTestDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabheemanadhuni/Downloads/hackathon/AutomationFramework/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7040EA40-4AD2-D145-8AE5-C37FE0A41201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A317B21F-8788-594A-8206-EDB0094115FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="1500" windowWidth="28040" windowHeight="17240" xr2:uid="{FFFCF1A5-D642-9B49-89EA-FE281DFFEC9E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>TestId</t>
   </si>
@@ -53,6 +53,27 @@
     <t>TC1</t>
   </si>
   <si>
+    <t>ERR-4004</t>
+  </si>
+  <si>
+    <t>Resource not found</t>
+  </si>
+  <si>
+    <t>FATAL - ERR-4004: Resource not found in module Tampflex. User: miles.schuster, SessionID: 292a6028-2064-46f1-98a4-2d90283bd12f</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>ERR-2002</t>
+  </si>
+  <si>
+    <t>Authentication failed</t>
+  </si>
+  <si>
+    <t>ERROR - ERR-2002: Authentication failed in module Otcom. User: curtis.lakin, SessionID: 1fdcd4c4-5740-467c-b533-2e00b3818c59</t>
+  </si>
+  <si>
     <t>ERR-5005</t>
   </si>
   <si>
@@ -62,16 +83,13 @@
     <t>ERROR - ERR-5005: Internal server error in module Hatity. User: kasie.ankunding, SessionID: 0f210e9c-8293-4087-bfed-98d284d7bc54</t>
   </si>
   <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>ERR-4004</t>
-  </si>
-  <si>
-    <t>Resource not found</t>
-  </si>
-  <si>
-    <t>FATAL - ERR-4004: Resource not found in module Tampflex. User: miles.schuster, SessionID: 292a6028-2064-46f1-98a4-2d90283bd12f</t>
+    <t>ERR-1001</t>
+  </si>
+  <si>
+    <t>connection timeout</t>
+  </si>
+  <si>
+    <t>WARN - ERR-1001: connection timeout in module Fixflex. User: nicky.stracke, SessionID: b92e0e36-d08c-4864-b072-bcf6b0a5868f</t>
   </si>
 </sst>
 </file>
@@ -447,10 +465,13 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" customWidth="true" width="30.33203125" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -471,13 +492,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -485,13 +506,13 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data clear in excel
</commit_message>
<xml_diff>
--- a/analysis/failedTestDetails.xlsx
+++ b/analysis/failedTestDetails.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>TestId</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>WARN - ERR-1001: connection timeout in module Fixflex. User: nicky.stracke, SessionID: b92e0e36-d08c-4864-b072-bcf6b0a5868f</t>
+  </si>
+  <si>
+    <t>ERR-3003</t>
+  </si>
+  <si>
+    <t>Invalid input parameter</t>
+  </si>
+  <si>
+    <t>WARN - ERR-3003: Invalid input parameter in module Tempsoft. User: kyle.windler, SessionID: 5f98e075-91e7-4882-bec8-79b4bb6920ea</t>
   </si>
 </sst>
 </file>
@@ -492,13 +501,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -506,13 +515,13 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>